<commit_message>
Packaging Meterial Data Base Update
</commit_message>
<xml_diff>
--- a/production_recipe_management_tool_v1.1/data/Packaging_Material_List.xlsx
+++ b/production_recipe_management_tool_v1.1/data/Packaging_Material_List.xlsx
@@ -1,20 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deborshi\Desktop\production_recipe_management_tool\production_recipe_management_tool_v1.1\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882E4FC0-2D1B-41C2-ADCD-2AC69E162C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>Product</t>
   </si>
@@ -31,38 +48,56 @@
     <t>Current Stock (Pieces)</t>
   </si>
   <si>
-    <t>Aluminum Foil</t>
-  </si>
-  <si>
-    <t>ABC1</t>
-  </si>
-  <si>
-    <t>ABC2</t>
-  </si>
-  <si>
-    <t>ABC3</t>
-  </si>
-  <si>
-    <t>ABC4</t>
-  </si>
-  <si>
-    <t>ABC5</t>
-  </si>
-  <si>
-    <t>ABC6</t>
-  </si>
-  <si>
     <t>gm</t>
   </si>
   <si>
     <t>Pieces</t>
+  </si>
+  <si>
+    <t>Brown Paper Bag 1</t>
+  </si>
+  <si>
+    <t>Brown Paper Bag 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 CP Container </t>
+  </si>
+  <si>
+    <t>100 ML Container Basic</t>
+  </si>
+  <si>
+    <t>300 ML Container</t>
+  </si>
+  <si>
+    <t>500 ML Container</t>
+  </si>
+  <si>
+    <t>750 ML Container</t>
+  </si>
+  <si>
+    <t>Tissues</t>
+  </si>
+  <si>
+    <t>500 ML Container Basic</t>
+  </si>
+  <si>
+    <t>300 ML Container Basic</t>
+  </si>
+  <si>
+    <t>750 ML Container Basic</t>
+  </si>
+  <si>
+    <t>Butter Paper</t>
+  </si>
+  <si>
+    <t>Non woven bag 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,24 +149,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -169,7 +213,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -203,6 +247,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -237,9 +282,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -412,14 +458,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:E16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,125 +487,276 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="D3" s="2">
+        <v>78</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>98</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2">
+        <v>23</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3.95</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>67</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2.95</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="2">
+        <f>20/1000</f>
+        <v>0.02</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2">
-        <v>0.5</v>
-      </c>
-      <c r="D2">
-        <v>45</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>0.8</v>
-      </c>
-      <c r="D3">
-        <v>78</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>0.1</v>
-      </c>
-      <c r="D4">
-        <v>98</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>0.75</v>
-      </c>
-      <c r="D5">
-        <v>23</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>0.75</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>0.58</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8">
-        <v>0.6767</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>67</v>
-      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>